<commit_message>
Automatize downloads for ILO and WHO
-WHO_data.R: downloads data from WHO
-ILO_data.R: downloads data from ILO
-clean_data.do: update the sections of WHO and ILO to match the data download with API (instead of uploading one excel for each indicator, take the complete excel. Use original names in the data)
</commit_message>
<xml_diff>
--- a/Data/Data_Raw/Country codes & metadata/wbcodes_equiv_who.xlsx
+++ b/Data/Data_Raw/Country codes & metadata/wbcodes_equiv_who.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laboral\World Bank\Data-Portal-Brief-Generator\Data\Data_Raw\Country codes &amp; metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alumniutdt-my.sharepoint.com/personal/yllohis_mail_utdt_edu/Documents/WB/Data-Portal-Brief-Generator/Data/Data_Raw/Country codes &amp; metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{044F24B9-041E-420A-A303-57252859EA49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{044F24B9-041E-420A-A303-57252859EA49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F110E60-3770-4130-8B2B-EBAD7611E44F}"/>
   <bookViews>
-    <workbookView xWindow="2124" yWindow="2124" windowWidth="17280" windowHeight="8964" xr2:uid="{57CC7407-EB43-432E-BADF-FE7D3FB84E50}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{57CC7407-EB43-432E-BADF-FE7D3FB84E50}"/>
   </bookViews>
   <sheets>
     <sheet name="WHO" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="455">
   <si>
     <t>WHO_code</t>
   </si>
@@ -1371,6 +1371,36 @@
   </si>
   <si>
     <t>Macao SAR</t>
+  </si>
+  <si>
+    <t>ASM</t>
+  </si>
+  <si>
+    <t>American Samoa</t>
+  </si>
+  <si>
+    <t>Bermuda</t>
+  </si>
+  <si>
+    <t>BMU</t>
+  </si>
+  <si>
+    <t>GRL</t>
+  </si>
+  <si>
+    <t>Greenland</t>
+  </si>
+  <si>
+    <t>PRI</t>
+  </si>
+  <si>
+    <t>Puerto Rico</t>
+  </si>
+  <si>
+    <t>PYF</t>
+  </si>
+  <si>
+    <t>French Polynesia</t>
   </si>
 </sst>
 </file>
@@ -1386,12 +1416,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1406,8 +1442,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1426,9 +1463,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1466,7 +1503,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1572,7 +1609,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1714,7 +1751,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1722,15 +1759,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA5C33FB-58EE-4907-96B2-D9F89823B59E}">
-  <dimension ref="A1:D206"/>
+  <dimension ref="A1:D211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A191" workbookViewId="0">
-      <selection activeCell="B207" sqref="B207"/>
+    <sheetView tabSelected="1" topLeftCell="A194" workbookViewId="0">
+      <selection activeCell="E202" sqref="E202"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1744,7 +1781,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1758,7 +1795,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1772,7 +1809,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1786,7 +1823,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1800,7 +1837,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1814,7 +1851,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1828,7 +1865,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1842,7 +1879,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1856,7 +1893,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1870,7 +1907,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -1884,7 +1921,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -1898,7 +1935,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1912,7 +1949,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -1926,7 +1963,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -1940,7 +1977,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -1954,7 +1991,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -1968,7 +2005,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -1982,7 +2019,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>40</v>
       </c>
@@ -1996,7 +2033,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -2010,7 +2047,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>44</v>
       </c>
@@ -2024,7 +2061,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>46</v>
       </c>
@@ -2038,7 +2075,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>48</v>
       </c>
@@ -2052,7 +2089,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>51</v>
       </c>
@@ -2066,7 +2103,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>53</v>
       </c>
@@ -2080,7 +2117,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>55</v>
       </c>
@@ -2094,7 +2131,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>57</v>
       </c>
@@ -2108,7 +2145,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>59</v>
       </c>
@@ -2122,7 +2159,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>62</v>
       </c>
@@ -2136,7 +2173,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>64</v>
       </c>
@@ -2150,7 +2187,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>66</v>
       </c>
@@ -2164,7 +2201,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>68</v>
       </c>
@@ -2178,7 +2215,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>71</v>
       </c>
@@ -2192,7 +2229,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>73</v>
       </c>
@@ -2206,7 +2243,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>75</v>
       </c>
@@ -2220,7 +2257,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>77</v>
       </c>
@@ -2234,7 +2271,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>79</v>
       </c>
@@ -2248,7 +2285,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>81</v>
       </c>
@@ -2262,7 +2299,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>83</v>
       </c>
@@ -2276,7 +2313,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>85</v>
       </c>
@@ -2290,7 +2327,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>87</v>
       </c>
@@ -2304,7 +2341,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>89</v>
       </c>
@@ -2318,7 +2355,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>92</v>
       </c>
@@ -2332,7 +2369,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>94</v>
       </c>
@@ -2346,7 +2383,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>96</v>
       </c>
@@ -2360,7 +2397,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>99</v>
       </c>
@@ -2374,7 +2411,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>101</v>
       </c>
@@ -2388,7 +2425,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>103</v>
       </c>
@@ -2402,7 +2439,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>105</v>
       </c>
@@ -2416,7 +2453,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>108</v>
       </c>
@@ -2430,7 +2467,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>111</v>
       </c>
@@ -2444,7 +2481,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>114</v>
       </c>
@@ -2458,7 +2495,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>116</v>
       </c>
@@ -2472,7 +2509,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>118</v>
       </c>
@@ -2486,7 +2523,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>120</v>
       </c>
@@ -2500,7 +2537,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>122</v>
       </c>
@@ -2514,7 +2551,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>124</v>
       </c>
@@ -2528,7 +2565,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>127</v>
       </c>
@@ -2542,7 +2579,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>129</v>
       </c>
@@ -2556,7 +2593,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>131</v>
       </c>
@@ -2570,7 +2607,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>133</v>
       </c>
@@ -2584,7 +2621,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>135</v>
       </c>
@@ -2598,7 +2635,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>138</v>
       </c>
@@ -2612,7 +2649,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>140</v>
       </c>
@@ -2626,7 +2663,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>142</v>
       </c>
@@ -2640,7 +2677,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>144</v>
       </c>
@@ -2654,7 +2691,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>146</v>
       </c>
@@ -2668,7 +2705,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>149</v>
       </c>
@@ -2682,7 +2719,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>151</v>
       </c>
@@ -2696,7 +2733,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>153</v>
       </c>
@@ -2710,7 +2747,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>155</v>
       </c>
@@ -2724,7 +2761,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>157</v>
       </c>
@@ -2738,7 +2775,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>159</v>
       </c>
@@ -2752,7 +2789,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>161</v>
       </c>
@@ -2766,7 +2803,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>163</v>
       </c>
@@ -2780,7 +2817,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>165</v>
       </c>
@@ -2794,7 +2831,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>167</v>
       </c>
@@ -2808,7 +2845,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>169</v>
       </c>
@@ -2822,7 +2859,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>171</v>
       </c>
@@ -2836,7 +2873,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>173</v>
       </c>
@@ -2850,7 +2887,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>175</v>
       </c>
@@ -2864,7 +2901,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>177</v>
       </c>
@@ -2878,7 +2915,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>179</v>
       </c>
@@ -2892,7 +2929,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>181</v>
       </c>
@@ -2906,7 +2943,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>184</v>
       </c>
@@ -2920,7 +2957,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>186</v>
       </c>
@@ -2934,7 +2971,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>188</v>
       </c>
@@ -2948,7 +2985,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>190</v>
       </c>
@@ -2962,7 +2999,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>192</v>
       </c>
@@ -2976,7 +3013,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>194</v>
       </c>
@@ -2990,7 +3027,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>196</v>
       </c>
@@ -3004,7 +3041,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>198</v>
       </c>
@@ -3018,7 +3055,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>200</v>
       </c>
@@ -3032,7 +3069,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>202</v>
       </c>
@@ -3046,7 +3083,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>204</v>
       </c>
@@ -3060,7 +3097,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>206</v>
       </c>
@@ -3074,7 +3111,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>209</v>
       </c>
@@ -3088,7 +3125,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>212</v>
       </c>
@@ -3102,7 +3139,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>214</v>
       </c>
@@ -3116,7 +3153,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>216</v>
       </c>
@@ -3130,7 +3167,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>218</v>
       </c>
@@ -3144,7 +3181,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>220</v>
       </c>
@@ -3158,7 +3195,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>222</v>
       </c>
@@ -3172,7 +3209,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>224</v>
       </c>
@@ -3186,7 +3223,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>226</v>
       </c>
@@ -3200,7 +3237,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>228</v>
       </c>
@@ -3214,7 +3251,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>230</v>
       </c>
@@ -3228,7 +3265,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>232</v>
       </c>
@@ -3242,7 +3279,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>234</v>
       </c>
@@ -3256,7 +3293,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>236</v>
       </c>
@@ -3270,7 +3307,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>238</v>
       </c>
@@ -3284,7 +3321,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>240</v>
       </c>
@@ -3298,7 +3335,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>242</v>
       </c>
@@ -3312,7 +3349,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>244</v>
       </c>
@@ -3326,7 +3363,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>246</v>
       </c>
@@ -3340,7 +3377,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>248</v>
       </c>
@@ -3354,7 +3391,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>251</v>
       </c>
@@ -3368,7 +3405,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>253</v>
       </c>
@@ -3382,7 +3419,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>255</v>
       </c>
@@ -3396,7 +3433,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>257</v>
       </c>
@@ -3410,7 +3447,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>259</v>
       </c>
@@ -3424,7 +3461,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>261</v>
       </c>
@@ -3438,7 +3475,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>263</v>
       </c>
@@ -3452,7 +3489,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>265</v>
       </c>
@@ -3466,7 +3503,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>267</v>
       </c>
@@ -3480,7 +3517,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>269</v>
       </c>
@@ -3494,7 +3531,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>271</v>
       </c>
@@ -3508,7 +3545,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>273</v>
       </c>
@@ -3522,7 +3559,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>275</v>
       </c>
@@ -3536,7 +3573,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>277</v>
       </c>
@@ -3550,7 +3587,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>279</v>
       </c>
@@ -3564,7 +3601,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>281</v>
       </c>
@@ -3578,7 +3615,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>283</v>
       </c>
@@ -3592,7 +3629,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>285</v>
       </c>
@@ -3606,7 +3643,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>287</v>
       </c>
@@ -3620,7 +3657,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>289</v>
       </c>
@@ -3634,7 +3671,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>291</v>
       </c>
@@ -3648,7 +3685,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>293</v>
       </c>
@@ -3662,7 +3699,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>295</v>
       </c>
@@ -3676,7 +3713,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>297</v>
       </c>
@@ -3690,7 +3727,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>299</v>
       </c>
@@ -3704,7 +3741,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>301</v>
       </c>
@@ -3718,7 +3755,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>303</v>
       </c>
@@ -3732,7 +3769,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>305</v>
       </c>
@@ -3746,7 +3783,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>307</v>
       </c>
@@ -3760,7 +3797,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>310</v>
       </c>
@@ -3774,7 +3811,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>313</v>
       </c>
@@ -3788,7 +3825,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>315</v>
       </c>
@@ -3802,7 +3839,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>317</v>
       </c>
@@ -3816,7 +3853,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>319</v>
       </c>
@@ -3830,7 +3867,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>322</v>
       </c>
@@ -3844,7 +3881,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>325</v>
       </c>
@@ -3858,7 +3895,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>328</v>
       </c>
@@ -3872,7 +3909,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>330</v>
       </c>
@@ -3886,7 +3923,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>332</v>
       </c>
@@ -3900,7 +3937,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>334</v>
       </c>
@@ -3914,7 +3951,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>336</v>
       </c>
@@ -3928,7 +3965,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>338</v>
       </c>
@@ -3942,7 +3979,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>340</v>
       </c>
@@ -3956,7 +3993,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>342</v>
       </c>
@@ -3970,7 +4007,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>344</v>
       </c>
@@ -3984,7 +4021,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>346</v>
       </c>
@@ -3998,7 +4035,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>349</v>
       </c>
@@ -4012,7 +4049,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>351</v>
       </c>
@@ -4026,7 +4063,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>353</v>
       </c>
@@ -4040,7 +4077,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>355</v>
       </c>
@@ -4054,7 +4091,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>357</v>
       </c>
@@ -4068,7 +4105,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>359</v>
       </c>
@@ -4082,7 +4119,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>361</v>
       </c>
@@ -4096,7 +4133,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>363</v>
       </c>
@@ -4110,7 +4147,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>365</v>
       </c>
@@ -4124,7 +4161,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>367</v>
       </c>
@@ -4138,7 +4175,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>369</v>
       </c>
@@ -4152,7 +4189,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>371</v>
       </c>
@@ -4166,7 +4203,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>373</v>
       </c>
@@ -4180,7 +4217,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>375</v>
       </c>
@@ -4194,7 +4231,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>377</v>
       </c>
@@ -4208,7 +4245,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>379</v>
       </c>
@@ -4222,7 +4259,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>381</v>
       </c>
@@ -4236,7 +4273,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>384</v>
       </c>
@@ -4250,7 +4287,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>386</v>
       </c>
@@ -4264,7 +4301,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>388</v>
       </c>
@@ -4278,7 +4315,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>390</v>
       </c>
@@ -4292,7 +4329,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>392</v>
       </c>
@@ -4306,7 +4343,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>394</v>
       </c>
@@ -4320,7 +4357,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>396</v>
       </c>
@@ -4334,7 +4371,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>398</v>
       </c>
@@ -4348,7 +4385,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>400</v>
       </c>
@@ -4362,7 +4399,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>403</v>
       </c>
@@ -4376,7 +4413,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>405</v>
       </c>
@@ -4390,7 +4427,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>407</v>
       </c>
@@ -4404,7 +4441,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>409</v>
       </c>
@@ -4418,7 +4455,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>411</v>
       </c>
@@ -4432,7 +4469,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>413</v>
       </c>
@@ -4446,7 +4483,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>416</v>
       </c>
@@ -4460,7 +4497,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>418</v>
       </c>
@@ -4474,7 +4511,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>420</v>
       </c>
@@ -4488,7 +4525,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>422</v>
       </c>
@@ -4502,7 +4539,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>424</v>
       </c>
@@ -4516,7 +4553,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>427</v>
       </c>
@@ -4530,7 +4567,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>430</v>
       </c>
@@ -4544,7 +4581,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>433</v>
       </c>
@@ -4558,7 +4595,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>435</v>
       </c>
@@ -4572,7 +4609,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>438</v>
       </c>
@@ -4586,7 +4623,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>441</v>
       </c>
@@ -4600,7 +4637,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>443</v>
       </c>
@@ -4612,6 +4649,76 @@
       </c>
       <c r="D206" t="s">
         <v>443</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A207" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="C207" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="D207" s="1" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A208" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="C208" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="D208" s="1" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A209" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="C209" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="D209" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A210" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="C210" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="D210" s="1" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A211" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="B211" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="C211" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="D211" s="1" t="s">
+        <v>453</v>
       </c>
     </row>
   </sheetData>

</xml_diff>